<commit_message>
Small correction of the database
Some codes of the conversion technologies were fixed in the database.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION_NEW.xlsx
+++ b/cea/databases/CH/components/CONVERSION_NEW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/CEA_Testing/reference-case-open/baseline/inputs/technology/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD116D76-1881-B643-804E-ECC501D796EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E087E3E-A3E1-2743-A9FC-117671AAB145}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="14860" windowWidth="25600" windowHeight="16000" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="993" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="photovoltaic_panels" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="218">
   <si>
     <t>Description</t>
   </si>
@@ -336,18 +336,6 @@
     <t>PU1</t>
   </si>
   <si>
-    <t>District substation heat exchanger</t>
-  </si>
-  <si>
-    <t>HEX2</t>
-  </si>
-  <si>
-    <t>m^2</t>
-  </si>
-  <si>
-    <t>Values under 1 and above 50 are assumptions, as no datasheet values are available in this area. a_p to e_p denote the pressure drop in Pa</t>
-  </si>
-  <si>
     <t>a_p</t>
   </si>
   <si>
@@ -639,9 +627,6 @@
     <t>counter-flow, plate</t>
   </si>
   <si>
-    <t>concurrent flow, tube</t>
-  </si>
-  <si>
     <t>T_max_operating</t>
   </si>
   <si>
@@ -703,6 +688,9 @@
   </si>
   <si>
     <t>air-source</t>
+  </si>
+  <si>
+    <t>BO3</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2375,7 +2363,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2399,7 +2387,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2411,16 +2399,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -2453,21 +2441,21 @@
         <v>26</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E2" s="2">
         <v>28000</v>
@@ -2521,21 +2509,21 @@
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E3" s="2">
         <v>90000</v>
@@ -2589,21 +2577,21 @@
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E4" s="2">
         <v>730000</v>
@@ -2657,21 +2645,21 @@
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E5" s="2">
         <v>28000</v>
@@ -2725,21 +2713,21 @@
       </c>
       <c r="U5" s="2"/>
       <c r="V5" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E6" s="2">
         <v>90000</v>
@@ -2793,21 +2781,21 @@
       </c>
       <c r="U6" s="2"/>
       <c r="V6" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E7" s="2">
         <v>730000</v>
@@ -2861,21 +2849,21 @@
       </c>
       <c r="U7" s="2"/>
       <c r="V7" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E8" s="2">
         <v>28000</v>
@@ -2929,21 +2917,21 @@
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E9" s="2">
         <v>90000</v>
@@ -2997,21 +2985,21 @@
       </c>
       <c r="U9" s="2"/>
       <c r="V9" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E10" s="2">
         <v>730000</v>
@@ -3065,7 +3053,7 @@
       </c>
       <c r="U10" s="2"/>
       <c r="V10" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3108,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E1" s="43" t="s">
         <v>3</v>
@@ -3120,19 +3108,19 @@
         <v>5</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I1" s="46" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K1" s="46" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M1" s="43" t="s">
         <v>17</v>
@@ -3165,21 +3153,21 @@
         <v>26</v>
       </c>
       <c r="W1" s="43" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E2" s="20">
         <v>850000</v>
@@ -3233,24 +3221,24 @@
         <v>5</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E3" s="20">
         <v>2600000</v>
@@ -3304,24 +3292,24 @@
         <v>5</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W3" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E4" s="31">
         <v>3500000</v>
@@ -3375,24 +3363,24 @@
         <v>5</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W4" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E5" s="32">
         <v>180000</v>
@@ -3446,24 +3434,24 @@
         <v>5</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W5" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E6" s="32">
         <v>280000</v>
@@ -3517,24 +3505,24 @@
         <v>5</v>
       </c>
       <c r="V6" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W6" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E7" s="32">
         <v>900000</v>
@@ -3588,24 +3576,24 @@
         <v>5</v>
       </c>
       <c r="V7" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="W7" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E8" s="32">
         <v>1000000</v>
@@ -3662,21 +3650,21 @@
         <v>84</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E9" s="32">
         <v>5000000</v>
@@ -3733,21 +3721,21 @@
         <v>84</v>
       </c>
       <c r="W9" s="34" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>197</v>
-      </c>
       <c r="C10" s="19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E10" s="32">
         <v>1000000</v>
@@ -3804,21 +3792,21 @@
         <v>84</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E11" s="32">
         <v>30000000</v>
@@ -3876,7 +3864,7 @@
         <v>84</v>
       </c>
       <c r="W11" s="34" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -4580,7 +4568,7 @@
         <v>23</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="O1" s="43" t="s">
         <v>24</v>
@@ -4589,31 +4577,31 @@
         <v>25</v>
       </c>
       <c r="Q1" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="U1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="43" t="s">
+      <c r="V1" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="W1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="43" t="s">
+      <c r="X1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="Y1" s="43" t="s">
         <v>114</v>
-      </c>
-      <c r="V1" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="W1" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="X1" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y1" s="43" t="s">
-        <v>118</v>
       </c>
       <c r="Z1" s="43" t="s">
         <v>26</v>
@@ -4627,7 +4615,7 @@
         <v>93</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
@@ -4709,7 +4697,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D3" s="2">
         <v>12000</v>
@@ -4785,13 +4773,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>96</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D4" s="12">
         <v>0</v>
@@ -4800,7 +4788,7 @@
         <v>10000000000</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>31</v>
@@ -4865,13 +4853,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
@@ -4880,7 +4868,7 @@
         <v>10000000000</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>31</v>
@@ -4945,13 +4933,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
@@ -4960,7 +4948,7 @@
         <v>10000000000</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>31</v>
@@ -5025,13 +5013,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
@@ -5040,7 +5028,7 @@
         <v>10000000000</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>31</v>
@@ -5105,13 +5093,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D8" s="12">
         <v>0</v>
@@ -5120,7 +5108,7 @@
         <v>10000000000</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>31</v>
@@ -6037,7 +6025,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="S1" sqref="Q1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6074,16 +6062,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K1" s="43" t="s">
         <v>17</v>
@@ -6116,18 +6104,18 @@
         <v>26</v>
       </c>
       <c r="U1" s="43" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="D2" s="21">
         <v>0</v>
@@ -6181,18 +6169,18 @@
         <v>84</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D3" s="20">
         <v>0</v>
@@ -6246,7 +6234,7 @@
         <v>84</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -6257,6 +6245,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6302,16 +6291,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K1" s="43" t="s">
         <v>17</v>
@@ -6344,18 +6333,18 @@
         <v>26</v>
       </c>
       <c r="U1" s="43" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D2" s="21">
         <v>1050000</v>
@@ -6406,21 +6395,21 @@
         <v>5</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D3" s="20">
         <v>1</v>
@@ -6476,18 +6465,18 @@
         <v>25</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D4" s="20">
         <v>260000</v>
@@ -6543,18 +6532,18 @@
         <v>25</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D5" s="20">
         <v>530000</v>
@@ -6610,18 +6599,18 @@
         <v>25</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D6" s="20">
         <v>1050000</v>
@@ -6677,18 +6666,18 @@
         <v>25</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D7" s="21">
         <v>2110000</v>
@@ -6742,7 +6731,7 @@
         <v>25</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -6799,22 +6788,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>17</v>
@@ -6877,12 +6866,12 @@
         <v>75</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>76</v>
@@ -6978,12 +6967,12 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>76</v>
@@ -7079,12 +7068,12 @@
         <v>33</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>78</v>
@@ -7180,12 +7169,12 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>78</v>
@@ -7281,12 +7270,12 @@
         <v>14</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>78</v>
@@ -7382,12 +7371,12 @@
         <v>14</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>79</v>
@@ -7536,19 +7525,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K1" s="43" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L1" s="43" t="s">
         <v>17</v>
@@ -7581,7 +7570,7 @@
         <v>26</v>
       </c>
       <c r="V1" s="47" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -7592,7 +7581,7 @@
         <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -7649,7 +7638,7 @@
         <v>84</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -7660,7 +7649,7 @@
         <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D3" s="2">
         <v>10000000</v>
@@ -7717,7 +7706,7 @@
         <v>84</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -7725,10 +7714,10 @@
         <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -7785,7 +7774,7 @@
         <v>24</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -7793,10 +7782,10 @@
         <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D5" s="2">
         <v>10000000</v>
@@ -7853,7 +7842,7 @@
         <v>84</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -7922,10 +7911,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7961,16 +7950,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K1" s="43" t="s">
         <v>17</v>
@@ -7991,19 +7980,19 @@
         <v>22</v>
       </c>
       <c r="Q1" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" s="43" t="s">
         <v>103</v>
-      </c>
-      <c r="R1" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="T1" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="U1" s="43" t="s">
-        <v>107</v>
       </c>
       <c r="V1" s="43" t="s">
         <v>23</v>
@@ -8018,7 +8007,7 @@
         <v>26</v>
       </c>
       <c r="Z1" s="47" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -8029,7 +8018,7 @@
         <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D2" s="2">
         <v>50000</v>
@@ -8047,10 +8036,10 @@
         <v>160</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>31</v>
@@ -8100,7 +8089,7 @@
         <v>84</v>
       </c>
       <c r="Z2" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -8111,7 +8100,7 @@
         <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D3" s="2">
         <v>80000</v>
@@ -8129,10 +8118,10 @@
         <v>160</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>31</v>
@@ -8181,7 +8170,7 @@
         <v>84</v>
       </c>
       <c r="Z3" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -8192,7 +8181,7 @@
         <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D4" s="2">
         <v>100000</v>
@@ -8210,10 +8199,10 @@
         <v>160</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>31</v>
@@ -8263,87 +8252,7 @@
         <v>84</v>
       </c>
       <c r="Z4" s="34" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>500</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-20</v>
-      </c>
-      <c r="H5" s="2">
-        <v>180</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="2">
-        <v>3381</v>
-      </c>
-      <c r="M5" s="2">
-        <v>229.8</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>5056</v>
-      </c>
-      <c r="R5" s="2">
-        <v>319.89999999999998</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0.4153</v>
-      </c>
-      <c r="T5" s="2">
-        <v>-1271</v>
-      </c>
-      <c r="U5" s="2">
-        <v>6.8329999999999997E-3</v>
-      </c>
-      <c r="V5" s="2">
-        <v>20</v>
-      </c>
-      <c r="W5" s="2">
-        <v>5</v>
-      </c>
-      <c r="X5" s="2">
-        <v>5</v>
-      </c>
-      <c r="Y5" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z5" s="34" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -8401,22 +8310,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H1" s="47" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I1" s="47" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J1" s="47" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K1" s="47" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="M1" s="45" t="s">
         <v>17</v>
@@ -8449,18 +8358,18 @@
         <v>26</v>
       </c>
       <c r="W1" s="47" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D2" s="20">
         <v>0</v>
@@ -8484,10 +8393,10 @@
         <v>27</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M2" s="26" t="s">
         <v>31</v>
@@ -8519,18 +8428,18 @@
       </c>
       <c r="V2" s="16"/>
       <c r="W2" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D3" s="21">
         <v>40000</v>
@@ -8554,10 +8463,10 @@
         <v>27</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M3" s="26" t="s">
         <v>31</v>
@@ -8589,18 +8498,18 @@
       </c>
       <c r="V3" s="16"/>
       <c r="W3" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D4" s="20">
         <v>0</v>
@@ -8624,10 +8533,10 @@
         <v>27</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M4" s="26" t="s">
         <v>31</v>
@@ -8660,18 +8569,18 @@
       </c>
       <c r="V4" s="16"/>
       <c r="W4" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D5" s="21">
         <v>21000</v>
@@ -8695,10 +8604,10 @@
         <v>27</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M5" s="26" t="s">
         <v>31</v>
@@ -8731,18 +8640,18 @@
       </c>
       <c r="V5" s="16"/>
       <c r="W5" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D6" s="20">
         <v>40000</v>
@@ -8766,10 +8675,10 @@
         <v>27</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M6" s="26" t="s">
         <v>31</v>
@@ -8802,18 +8711,18 @@
       </c>
       <c r="V6" s="16"/>
       <c r="W6" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D7" s="21">
         <v>75000</v>
@@ -8837,10 +8746,10 @@
         <v>27</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>31</v>
@@ -8873,18 +8782,18 @@
       </c>
       <c r="V7" s="16"/>
       <c r="W7" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D8" s="20">
         <v>0</v>
@@ -8908,10 +8817,10 @@
         <v>35</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M8" s="26" t="s">
         <v>31</v>
@@ -8942,21 +8851,21 @@
         <v>6</v>
       </c>
       <c r="V8" s="16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D9" s="21">
         <v>21000</v>
@@ -8980,10 +8889,10 @@
         <v>35</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M9" s="26" t="s">
         <v>31</v>
@@ -9014,21 +8923,21 @@
         <v>6</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="W9" s="34" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D10" s="20">
         <v>40000</v>
@@ -9052,10 +8961,10 @@
         <v>35</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M10" s="26" t="s">
         <v>31</v>
@@ -9086,21 +8995,21 @@
         <v>6</v>
       </c>
       <c r="V10" s="16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D11" s="21">
         <v>75000</v>
@@ -9124,10 +9033,10 @@
         <v>35</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M11" s="26" t="s">
         <v>31</v>
@@ -9158,10 +9067,10 @@
         <v>6</v>
       </c>
       <c r="V11" s="16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="W11" s="34" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update databases one last time
lowered minimum capacity of some components, to allow for an adequate supply system component to be installed in small stand-alone buildings.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION_NEW.xlsx
+++ b/cea/databases/CH/components/CONVERSION_NEW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/CEA_Testing/reference-case-open/baseline/inputs/technology/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\CEA_Testing\heating_test\Austrasse\inputs\technology\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727BFB31-6FC0-154E-9478-51D085C5F01A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5100204A-78B3-4897-8B54-338C07A6C02B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="11780" windowWidth="25600" windowHeight="16000" tabRatio="993" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16780" windowHeight="5800" tabRatio="993" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="photovoltaic_panels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="__xlfn_AGGREGATE">#N/A</definedName>
     <definedName name="__xlfn_STDEV_S">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -1532,29 +1532,29 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.6328125" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.5" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" customWidth="1"/>
-    <col min="16" max="17" width="12.5" customWidth="1"/>
-    <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="23" width="10.5" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" customWidth="1"/>
-    <col min="27" max="27" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="8.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" customWidth="1"/>
+    <col min="15" max="15" width="14.6328125" customWidth="1"/>
+    <col min="16" max="17" width="12.453125" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" customWidth="1"/>
+    <col min="20" max="20" width="13.6328125" customWidth="1"/>
+    <col min="21" max="23" width="10.453125" customWidth="1"/>
+    <col min="24" max="24" width="14.6328125" customWidth="1"/>
+    <col min="25" max="25" width="12.6328125" customWidth="1"/>
+    <col min="27" max="27" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2409,20 +2409,20 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.5" customWidth="1"/>
-    <col min="22" max="22" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="72.5" customWidth="1"/>
+    <col min="6" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.6328125" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="72.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>179</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>179</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>179</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>178</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>178</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>178</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>183</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>183</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>184</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>186</v>
       </c>
@@ -3220,651 +3220,651 @@
       <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="5" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="5" width="19.36328125" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" customWidth="1"/>
-    <col min="26" max="26" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="43.33203125" customWidth="1"/>
-    <col min="258" max="258" width="12.6640625" customWidth="1"/>
-    <col min="259" max="259" width="19.6640625" customWidth="1"/>
-    <col min="260" max="261" width="19.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="43.36328125" customWidth="1"/>
+    <col min="258" max="258" width="12.6328125" customWidth="1"/>
+    <col min="259" max="259" width="19.6328125" customWidth="1"/>
+    <col min="260" max="261" width="19.36328125" customWidth="1"/>
     <col min="270" max="270" width="10" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="274" max="274" width="10" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="280" max="280" width="7" customWidth="1"/>
-    <col min="282" max="282" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="43.33203125" customWidth="1"/>
-    <col min="514" max="514" width="12.6640625" customWidth="1"/>
-    <col min="515" max="515" width="19.6640625" customWidth="1"/>
-    <col min="516" max="517" width="19.33203125" customWidth="1"/>
+    <col min="282" max="282" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="43.36328125" customWidth="1"/>
+    <col min="514" max="514" width="12.6328125" customWidth="1"/>
+    <col min="515" max="515" width="19.6328125" customWidth="1"/>
+    <col min="516" max="517" width="19.36328125" customWidth="1"/>
     <col min="526" max="526" width="10" bestFit="1" customWidth="1"/>
-    <col min="527" max="527" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="527" max="527" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="530" max="530" width="10" bestFit="1" customWidth="1"/>
-    <col min="534" max="534" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="534" max="534" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="536" max="536" width="7" customWidth="1"/>
-    <col min="538" max="538" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="43.33203125" customWidth="1"/>
-    <col min="770" max="770" width="12.6640625" customWidth="1"/>
-    <col min="771" max="771" width="19.6640625" customWidth="1"/>
-    <col min="772" max="773" width="19.33203125" customWidth="1"/>
+    <col min="538" max="538" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="43.36328125" customWidth="1"/>
+    <col min="770" max="770" width="12.6328125" customWidth="1"/>
+    <col min="771" max="771" width="19.6328125" customWidth="1"/>
+    <col min="772" max="773" width="19.36328125" customWidth="1"/>
     <col min="782" max="782" width="10" bestFit="1" customWidth="1"/>
-    <col min="783" max="783" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="783" max="783" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="786" max="786" width="10" bestFit="1" customWidth="1"/>
-    <col min="790" max="790" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="790" max="790" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="792" max="792" width="7" customWidth="1"/>
-    <col min="794" max="794" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="43.33203125" customWidth="1"/>
-    <col min="1026" max="1026" width="12.6640625" customWidth="1"/>
-    <col min="1027" max="1027" width="19.6640625" customWidth="1"/>
-    <col min="1028" max="1029" width="19.33203125" customWidth="1"/>
+    <col min="794" max="794" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="43.36328125" customWidth="1"/>
+    <col min="1026" max="1026" width="12.6328125" customWidth="1"/>
+    <col min="1027" max="1027" width="19.6328125" customWidth="1"/>
+    <col min="1028" max="1029" width="19.36328125" customWidth="1"/>
     <col min="1038" max="1038" width="10" bestFit="1" customWidth="1"/>
-    <col min="1039" max="1039" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1039" max="1039" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1042" max="1042" width="10" bestFit="1" customWidth="1"/>
-    <col min="1046" max="1046" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1046" max="1046" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1048" max="1048" width="7" customWidth="1"/>
-    <col min="1050" max="1050" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="43.33203125" customWidth="1"/>
-    <col min="1282" max="1282" width="12.6640625" customWidth="1"/>
-    <col min="1283" max="1283" width="19.6640625" customWidth="1"/>
-    <col min="1284" max="1285" width="19.33203125" customWidth="1"/>
+    <col min="1050" max="1050" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="43.36328125" customWidth="1"/>
+    <col min="1282" max="1282" width="12.6328125" customWidth="1"/>
+    <col min="1283" max="1283" width="19.6328125" customWidth="1"/>
+    <col min="1284" max="1285" width="19.36328125" customWidth="1"/>
     <col min="1294" max="1294" width="10" bestFit="1" customWidth="1"/>
-    <col min="1295" max="1295" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1295" max="1295" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1298" max="1298" width="10" bestFit="1" customWidth="1"/>
-    <col min="1302" max="1302" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1302" max="1302" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1304" max="1304" width="7" customWidth="1"/>
-    <col min="1306" max="1306" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="43.33203125" customWidth="1"/>
-    <col min="1538" max="1538" width="12.6640625" customWidth="1"/>
-    <col min="1539" max="1539" width="19.6640625" customWidth="1"/>
-    <col min="1540" max="1541" width="19.33203125" customWidth="1"/>
+    <col min="1306" max="1306" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="43.36328125" customWidth="1"/>
+    <col min="1538" max="1538" width="12.6328125" customWidth="1"/>
+    <col min="1539" max="1539" width="19.6328125" customWidth="1"/>
+    <col min="1540" max="1541" width="19.36328125" customWidth="1"/>
     <col min="1550" max="1550" width="10" bestFit="1" customWidth="1"/>
-    <col min="1551" max="1551" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1551" max="1551" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1554" max="1554" width="10" bestFit="1" customWidth="1"/>
-    <col min="1558" max="1558" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1558" max="1558" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1560" max="1560" width="7" customWidth="1"/>
-    <col min="1562" max="1562" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="43.33203125" customWidth="1"/>
-    <col min="1794" max="1794" width="12.6640625" customWidth="1"/>
-    <col min="1795" max="1795" width="19.6640625" customWidth="1"/>
-    <col min="1796" max="1797" width="19.33203125" customWidth="1"/>
+    <col min="1562" max="1562" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="43.36328125" customWidth="1"/>
+    <col min="1794" max="1794" width="12.6328125" customWidth="1"/>
+    <col min="1795" max="1795" width="19.6328125" customWidth="1"/>
+    <col min="1796" max="1797" width="19.36328125" customWidth="1"/>
     <col min="1806" max="1806" width="10" bestFit="1" customWidth="1"/>
-    <col min="1807" max="1807" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1807" max="1807" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1810" max="1810" width="10" bestFit="1" customWidth="1"/>
-    <col min="1814" max="1814" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1814" max="1814" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1816" max="1816" width="7" customWidth="1"/>
-    <col min="1818" max="1818" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="43.33203125" customWidth="1"/>
-    <col min="2050" max="2050" width="12.6640625" customWidth="1"/>
-    <col min="2051" max="2051" width="19.6640625" customWidth="1"/>
-    <col min="2052" max="2053" width="19.33203125" customWidth="1"/>
+    <col min="1818" max="1818" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="43.36328125" customWidth="1"/>
+    <col min="2050" max="2050" width="12.6328125" customWidth="1"/>
+    <col min="2051" max="2051" width="19.6328125" customWidth="1"/>
+    <col min="2052" max="2053" width="19.36328125" customWidth="1"/>
     <col min="2062" max="2062" width="10" bestFit="1" customWidth="1"/>
-    <col min="2063" max="2063" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2063" max="2063" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2066" max="2066" width="10" bestFit="1" customWidth="1"/>
-    <col min="2070" max="2070" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2070" max="2070" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2072" max="2072" width="7" customWidth="1"/>
-    <col min="2074" max="2074" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="43.33203125" customWidth="1"/>
-    <col min="2306" max="2306" width="12.6640625" customWidth="1"/>
-    <col min="2307" max="2307" width="19.6640625" customWidth="1"/>
-    <col min="2308" max="2309" width="19.33203125" customWidth="1"/>
+    <col min="2074" max="2074" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="43.36328125" customWidth="1"/>
+    <col min="2306" max="2306" width="12.6328125" customWidth="1"/>
+    <col min="2307" max="2307" width="19.6328125" customWidth="1"/>
+    <col min="2308" max="2309" width="19.36328125" customWidth="1"/>
     <col min="2318" max="2318" width="10" bestFit="1" customWidth="1"/>
-    <col min="2319" max="2319" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2319" max="2319" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2322" max="2322" width="10" bestFit="1" customWidth="1"/>
-    <col min="2326" max="2326" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2326" max="2326" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2328" max="2328" width="7" customWidth="1"/>
-    <col min="2330" max="2330" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="43.33203125" customWidth="1"/>
-    <col min="2562" max="2562" width="12.6640625" customWidth="1"/>
-    <col min="2563" max="2563" width="19.6640625" customWidth="1"/>
-    <col min="2564" max="2565" width="19.33203125" customWidth="1"/>
+    <col min="2330" max="2330" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="43.36328125" customWidth="1"/>
+    <col min="2562" max="2562" width="12.6328125" customWidth="1"/>
+    <col min="2563" max="2563" width="19.6328125" customWidth="1"/>
+    <col min="2564" max="2565" width="19.36328125" customWidth="1"/>
     <col min="2574" max="2574" width="10" bestFit="1" customWidth="1"/>
-    <col min="2575" max="2575" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2575" max="2575" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2578" max="2578" width="10" bestFit="1" customWidth="1"/>
-    <col min="2582" max="2582" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2582" max="2582" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2584" max="2584" width="7" customWidth="1"/>
-    <col min="2586" max="2586" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="43.33203125" customWidth="1"/>
-    <col min="2818" max="2818" width="12.6640625" customWidth="1"/>
-    <col min="2819" max="2819" width="19.6640625" customWidth="1"/>
-    <col min="2820" max="2821" width="19.33203125" customWidth="1"/>
+    <col min="2586" max="2586" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="43.36328125" customWidth="1"/>
+    <col min="2818" max="2818" width="12.6328125" customWidth="1"/>
+    <col min="2819" max="2819" width="19.6328125" customWidth="1"/>
+    <col min="2820" max="2821" width="19.36328125" customWidth="1"/>
     <col min="2830" max="2830" width="10" bestFit="1" customWidth="1"/>
-    <col min="2831" max="2831" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2831" max="2831" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2834" max="2834" width="10" bestFit="1" customWidth="1"/>
-    <col min="2838" max="2838" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2838" max="2838" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2840" max="2840" width="7" customWidth="1"/>
-    <col min="2842" max="2842" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="43.33203125" customWidth="1"/>
-    <col min="3074" max="3074" width="12.6640625" customWidth="1"/>
-    <col min="3075" max="3075" width="19.6640625" customWidth="1"/>
-    <col min="3076" max="3077" width="19.33203125" customWidth="1"/>
+    <col min="2842" max="2842" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="43.36328125" customWidth="1"/>
+    <col min="3074" max="3074" width="12.6328125" customWidth="1"/>
+    <col min="3075" max="3075" width="19.6328125" customWidth="1"/>
+    <col min="3076" max="3077" width="19.36328125" customWidth="1"/>
     <col min="3086" max="3086" width="10" bestFit="1" customWidth="1"/>
-    <col min="3087" max="3087" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3087" max="3087" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3090" max="3090" width="10" bestFit="1" customWidth="1"/>
-    <col min="3094" max="3094" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3094" max="3094" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3096" max="3096" width="7" customWidth="1"/>
-    <col min="3098" max="3098" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="43.33203125" customWidth="1"/>
-    <col min="3330" max="3330" width="12.6640625" customWidth="1"/>
-    <col min="3331" max="3331" width="19.6640625" customWidth="1"/>
-    <col min="3332" max="3333" width="19.33203125" customWidth="1"/>
+    <col min="3098" max="3098" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="43.36328125" customWidth="1"/>
+    <col min="3330" max="3330" width="12.6328125" customWidth="1"/>
+    <col min="3331" max="3331" width="19.6328125" customWidth="1"/>
+    <col min="3332" max="3333" width="19.36328125" customWidth="1"/>
     <col min="3342" max="3342" width="10" bestFit="1" customWidth="1"/>
-    <col min="3343" max="3343" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3343" max="3343" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3346" max="3346" width="10" bestFit="1" customWidth="1"/>
-    <col min="3350" max="3350" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3350" max="3350" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3352" max="3352" width="7" customWidth="1"/>
-    <col min="3354" max="3354" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="43.33203125" customWidth="1"/>
-    <col min="3586" max="3586" width="12.6640625" customWidth="1"/>
-    <col min="3587" max="3587" width="19.6640625" customWidth="1"/>
-    <col min="3588" max="3589" width="19.33203125" customWidth="1"/>
+    <col min="3354" max="3354" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="43.36328125" customWidth="1"/>
+    <col min="3586" max="3586" width="12.6328125" customWidth="1"/>
+    <col min="3587" max="3587" width="19.6328125" customWidth="1"/>
+    <col min="3588" max="3589" width="19.36328125" customWidth="1"/>
     <col min="3598" max="3598" width="10" bestFit="1" customWidth="1"/>
-    <col min="3599" max="3599" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3599" max="3599" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3602" max="3602" width="10" bestFit="1" customWidth="1"/>
-    <col min="3606" max="3606" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3606" max="3606" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3608" max="3608" width="7" customWidth="1"/>
-    <col min="3610" max="3610" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="43.33203125" customWidth="1"/>
-    <col min="3842" max="3842" width="12.6640625" customWidth="1"/>
-    <col min="3843" max="3843" width="19.6640625" customWidth="1"/>
-    <col min="3844" max="3845" width="19.33203125" customWidth="1"/>
+    <col min="3610" max="3610" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="43.36328125" customWidth="1"/>
+    <col min="3842" max="3842" width="12.6328125" customWidth="1"/>
+    <col min="3843" max="3843" width="19.6328125" customWidth="1"/>
+    <col min="3844" max="3845" width="19.36328125" customWidth="1"/>
     <col min="3854" max="3854" width="10" bestFit="1" customWidth="1"/>
-    <col min="3855" max="3855" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3855" max="3855" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3858" max="3858" width="10" bestFit="1" customWidth="1"/>
-    <col min="3862" max="3862" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3862" max="3862" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3864" max="3864" width="7" customWidth="1"/>
-    <col min="3866" max="3866" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="43.33203125" customWidth="1"/>
-    <col min="4098" max="4098" width="12.6640625" customWidth="1"/>
-    <col min="4099" max="4099" width="19.6640625" customWidth="1"/>
-    <col min="4100" max="4101" width="19.33203125" customWidth="1"/>
+    <col min="3866" max="3866" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="43.36328125" customWidth="1"/>
+    <col min="4098" max="4098" width="12.6328125" customWidth="1"/>
+    <col min="4099" max="4099" width="19.6328125" customWidth="1"/>
+    <col min="4100" max="4101" width="19.36328125" customWidth="1"/>
     <col min="4110" max="4110" width="10" bestFit="1" customWidth="1"/>
-    <col min="4111" max="4111" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4111" max="4111" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4114" max="4114" width="10" bestFit="1" customWidth="1"/>
-    <col min="4118" max="4118" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4118" max="4118" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4120" max="4120" width="7" customWidth="1"/>
-    <col min="4122" max="4122" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="43.33203125" customWidth="1"/>
-    <col min="4354" max="4354" width="12.6640625" customWidth="1"/>
-    <col min="4355" max="4355" width="19.6640625" customWidth="1"/>
-    <col min="4356" max="4357" width="19.33203125" customWidth="1"/>
+    <col min="4122" max="4122" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="43.36328125" customWidth="1"/>
+    <col min="4354" max="4354" width="12.6328125" customWidth="1"/>
+    <col min="4355" max="4355" width="19.6328125" customWidth="1"/>
+    <col min="4356" max="4357" width="19.36328125" customWidth="1"/>
     <col min="4366" max="4366" width="10" bestFit="1" customWidth="1"/>
-    <col min="4367" max="4367" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4367" max="4367" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4370" max="4370" width="10" bestFit="1" customWidth="1"/>
-    <col min="4374" max="4374" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4374" max="4374" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4376" max="4376" width="7" customWidth="1"/>
-    <col min="4378" max="4378" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="43.33203125" customWidth="1"/>
-    <col min="4610" max="4610" width="12.6640625" customWidth="1"/>
-    <col min="4611" max="4611" width="19.6640625" customWidth="1"/>
-    <col min="4612" max="4613" width="19.33203125" customWidth="1"/>
+    <col min="4378" max="4378" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="43.36328125" customWidth="1"/>
+    <col min="4610" max="4610" width="12.6328125" customWidth="1"/>
+    <col min="4611" max="4611" width="19.6328125" customWidth="1"/>
+    <col min="4612" max="4613" width="19.36328125" customWidth="1"/>
     <col min="4622" max="4622" width="10" bestFit="1" customWidth="1"/>
-    <col min="4623" max="4623" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4623" max="4623" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4626" max="4626" width="10" bestFit="1" customWidth="1"/>
-    <col min="4630" max="4630" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4630" max="4630" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4632" max="4632" width="7" customWidth="1"/>
-    <col min="4634" max="4634" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="43.33203125" customWidth="1"/>
-    <col min="4866" max="4866" width="12.6640625" customWidth="1"/>
-    <col min="4867" max="4867" width="19.6640625" customWidth="1"/>
-    <col min="4868" max="4869" width="19.33203125" customWidth="1"/>
+    <col min="4634" max="4634" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="43.36328125" customWidth="1"/>
+    <col min="4866" max="4866" width="12.6328125" customWidth="1"/>
+    <col min="4867" max="4867" width="19.6328125" customWidth="1"/>
+    <col min="4868" max="4869" width="19.36328125" customWidth="1"/>
     <col min="4878" max="4878" width="10" bestFit="1" customWidth="1"/>
-    <col min="4879" max="4879" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4879" max="4879" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4882" max="4882" width="10" bestFit="1" customWidth="1"/>
-    <col min="4886" max="4886" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4886" max="4886" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4888" max="4888" width="7" customWidth="1"/>
-    <col min="4890" max="4890" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="43.33203125" customWidth="1"/>
-    <col min="5122" max="5122" width="12.6640625" customWidth="1"/>
-    <col min="5123" max="5123" width="19.6640625" customWidth="1"/>
-    <col min="5124" max="5125" width="19.33203125" customWidth="1"/>
+    <col min="4890" max="4890" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="43.36328125" customWidth="1"/>
+    <col min="5122" max="5122" width="12.6328125" customWidth="1"/>
+    <col min="5123" max="5123" width="19.6328125" customWidth="1"/>
+    <col min="5124" max="5125" width="19.36328125" customWidth="1"/>
     <col min="5134" max="5134" width="10" bestFit="1" customWidth="1"/>
-    <col min="5135" max="5135" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5135" max="5135" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5138" max="5138" width="10" bestFit="1" customWidth="1"/>
-    <col min="5142" max="5142" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5142" max="5142" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5144" max="5144" width="7" customWidth="1"/>
-    <col min="5146" max="5146" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="43.33203125" customWidth="1"/>
-    <col min="5378" max="5378" width="12.6640625" customWidth="1"/>
-    <col min="5379" max="5379" width="19.6640625" customWidth="1"/>
-    <col min="5380" max="5381" width="19.33203125" customWidth="1"/>
+    <col min="5146" max="5146" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="43.36328125" customWidth="1"/>
+    <col min="5378" max="5378" width="12.6328125" customWidth="1"/>
+    <col min="5379" max="5379" width="19.6328125" customWidth="1"/>
+    <col min="5380" max="5381" width="19.36328125" customWidth="1"/>
     <col min="5390" max="5390" width="10" bestFit="1" customWidth="1"/>
-    <col min="5391" max="5391" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5391" max="5391" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5394" max="5394" width="10" bestFit="1" customWidth="1"/>
-    <col min="5398" max="5398" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5398" max="5398" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5400" max="5400" width="7" customWidth="1"/>
-    <col min="5402" max="5402" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="43.33203125" customWidth="1"/>
-    <col min="5634" max="5634" width="12.6640625" customWidth="1"/>
-    <col min="5635" max="5635" width="19.6640625" customWidth="1"/>
-    <col min="5636" max="5637" width="19.33203125" customWidth="1"/>
+    <col min="5402" max="5402" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="43.36328125" customWidth="1"/>
+    <col min="5634" max="5634" width="12.6328125" customWidth="1"/>
+    <col min="5635" max="5635" width="19.6328125" customWidth="1"/>
+    <col min="5636" max="5637" width="19.36328125" customWidth="1"/>
     <col min="5646" max="5646" width="10" bestFit="1" customWidth="1"/>
-    <col min="5647" max="5647" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5647" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5650" max="5650" width="10" bestFit="1" customWidth="1"/>
-    <col min="5654" max="5654" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5654" max="5654" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5656" max="5656" width="7" customWidth="1"/>
-    <col min="5658" max="5658" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="43.33203125" customWidth="1"/>
-    <col min="5890" max="5890" width="12.6640625" customWidth="1"/>
-    <col min="5891" max="5891" width="19.6640625" customWidth="1"/>
-    <col min="5892" max="5893" width="19.33203125" customWidth="1"/>
+    <col min="5658" max="5658" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="43.36328125" customWidth="1"/>
+    <col min="5890" max="5890" width="12.6328125" customWidth="1"/>
+    <col min="5891" max="5891" width="19.6328125" customWidth="1"/>
+    <col min="5892" max="5893" width="19.36328125" customWidth="1"/>
     <col min="5902" max="5902" width="10" bestFit="1" customWidth="1"/>
-    <col min="5903" max="5903" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5903" max="5903" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5906" max="5906" width="10" bestFit="1" customWidth="1"/>
-    <col min="5910" max="5910" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5910" max="5910" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5912" max="5912" width="7" customWidth="1"/>
-    <col min="5914" max="5914" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="43.33203125" customWidth="1"/>
-    <col min="6146" max="6146" width="12.6640625" customWidth="1"/>
-    <col min="6147" max="6147" width="19.6640625" customWidth="1"/>
-    <col min="6148" max="6149" width="19.33203125" customWidth="1"/>
+    <col min="5914" max="5914" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="43.36328125" customWidth="1"/>
+    <col min="6146" max="6146" width="12.6328125" customWidth="1"/>
+    <col min="6147" max="6147" width="19.6328125" customWidth="1"/>
+    <col min="6148" max="6149" width="19.36328125" customWidth="1"/>
     <col min="6158" max="6158" width="10" bestFit="1" customWidth="1"/>
-    <col min="6159" max="6159" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6159" max="6159" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6162" max="6162" width="10" bestFit="1" customWidth="1"/>
-    <col min="6166" max="6166" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6166" max="6166" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6168" max="6168" width="7" customWidth="1"/>
-    <col min="6170" max="6170" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="43.33203125" customWidth="1"/>
-    <col min="6402" max="6402" width="12.6640625" customWidth="1"/>
-    <col min="6403" max="6403" width="19.6640625" customWidth="1"/>
-    <col min="6404" max="6405" width="19.33203125" customWidth="1"/>
+    <col min="6170" max="6170" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="43.36328125" customWidth="1"/>
+    <col min="6402" max="6402" width="12.6328125" customWidth="1"/>
+    <col min="6403" max="6403" width="19.6328125" customWidth="1"/>
+    <col min="6404" max="6405" width="19.36328125" customWidth="1"/>
     <col min="6414" max="6414" width="10" bestFit="1" customWidth="1"/>
-    <col min="6415" max="6415" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6415" max="6415" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6418" max="6418" width="10" bestFit="1" customWidth="1"/>
-    <col min="6422" max="6422" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6422" max="6422" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6424" max="6424" width="7" customWidth="1"/>
-    <col min="6426" max="6426" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="43.33203125" customWidth="1"/>
-    <col min="6658" max="6658" width="12.6640625" customWidth="1"/>
-    <col min="6659" max="6659" width="19.6640625" customWidth="1"/>
-    <col min="6660" max="6661" width="19.33203125" customWidth="1"/>
+    <col min="6426" max="6426" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="43.36328125" customWidth="1"/>
+    <col min="6658" max="6658" width="12.6328125" customWidth="1"/>
+    <col min="6659" max="6659" width="19.6328125" customWidth="1"/>
+    <col min="6660" max="6661" width="19.36328125" customWidth="1"/>
     <col min="6670" max="6670" width="10" bestFit="1" customWidth="1"/>
-    <col min="6671" max="6671" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6671" max="6671" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6674" max="6674" width="10" bestFit="1" customWidth="1"/>
-    <col min="6678" max="6678" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6678" max="6678" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6680" max="6680" width="7" customWidth="1"/>
-    <col min="6682" max="6682" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="43.33203125" customWidth="1"/>
-    <col min="6914" max="6914" width="12.6640625" customWidth="1"/>
-    <col min="6915" max="6915" width="19.6640625" customWidth="1"/>
-    <col min="6916" max="6917" width="19.33203125" customWidth="1"/>
+    <col min="6682" max="6682" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="43.36328125" customWidth="1"/>
+    <col min="6914" max="6914" width="12.6328125" customWidth="1"/>
+    <col min="6915" max="6915" width="19.6328125" customWidth="1"/>
+    <col min="6916" max="6917" width="19.36328125" customWidth="1"/>
     <col min="6926" max="6926" width="10" bestFit="1" customWidth="1"/>
-    <col min="6927" max="6927" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6927" max="6927" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6930" max="6930" width="10" bestFit="1" customWidth="1"/>
-    <col min="6934" max="6934" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6934" max="6934" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6936" max="6936" width="7" customWidth="1"/>
-    <col min="6938" max="6938" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="43.33203125" customWidth="1"/>
-    <col min="7170" max="7170" width="12.6640625" customWidth="1"/>
-    <col min="7171" max="7171" width="19.6640625" customWidth="1"/>
-    <col min="7172" max="7173" width="19.33203125" customWidth="1"/>
+    <col min="6938" max="6938" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="43.36328125" customWidth="1"/>
+    <col min="7170" max="7170" width="12.6328125" customWidth="1"/>
+    <col min="7171" max="7171" width="19.6328125" customWidth="1"/>
+    <col min="7172" max="7173" width="19.36328125" customWidth="1"/>
     <col min="7182" max="7182" width="10" bestFit="1" customWidth="1"/>
-    <col min="7183" max="7183" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7183" max="7183" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7186" max="7186" width="10" bestFit="1" customWidth="1"/>
-    <col min="7190" max="7190" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7190" max="7190" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7192" max="7192" width="7" customWidth="1"/>
-    <col min="7194" max="7194" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="43.33203125" customWidth="1"/>
-    <col min="7426" max="7426" width="12.6640625" customWidth="1"/>
-    <col min="7427" max="7427" width="19.6640625" customWidth="1"/>
-    <col min="7428" max="7429" width="19.33203125" customWidth="1"/>
+    <col min="7194" max="7194" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="43.36328125" customWidth="1"/>
+    <col min="7426" max="7426" width="12.6328125" customWidth="1"/>
+    <col min="7427" max="7427" width="19.6328125" customWidth="1"/>
+    <col min="7428" max="7429" width="19.36328125" customWidth="1"/>
     <col min="7438" max="7438" width="10" bestFit="1" customWidth="1"/>
-    <col min="7439" max="7439" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7439" max="7439" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7442" max="7442" width="10" bestFit="1" customWidth="1"/>
-    <col min="7446" max="7446" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7446" max="7446" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7448" max="7448" width="7" customWidth="1"/>
-    <col min="7450" max="7450" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="43.33203125" customWidth="1"/>
-    <col min="7682" max="7682" width="12.6640625" customWidth="1"/>
-    <col min="7683" max="7683" width="19.6640625" customWidth="1"/>
-    <col min="7684" max="7685" width="19.33203125" customWidth="1"/>
+    <col min="7450" max="7450" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="43.36328125" customWidth="1"/>
+    <col min="7682" max="7682" width="12.6328125" customWidth="1"/>
+    <col min="7683" max="7683" width="19.6328125" customWidth="1"/>
+    <col min="7684" max="7685" width="19.36328125" customWidth="1"/>
     <col min="7694" max="7694" width="10" bestFit="1" customWidth="1"/>
-    <col min="7695" max="7695" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7695" max="7695" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7698" max="7698" width="10" bestFit="1" customWidth="1"/>
-    <col min="7702" max="7702" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7702" max="7702" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7704" max="7704" width="7" customWidth="1"/>
-    <col min="7706" max="7706" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="43.33203125" customWidth="1"/>
-    <col min="7938" max="7938" width="12.6640625" customWidth="1"/>
-    <col min="7939" max="7939" width="19.6640625" customWidth="1"/>
-    <col min="7940" max="7941" width="19.33203125" customWidth="1"/>
+    <col min="7706" max="7706" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="43.36328125" customWidth="1"/>
+    <col min="7938" max="7938" width="12.6328125" customWidth="1"/>
+    <col min="7939" max="7939" width="19.6328125" customWidth="1"/>
+    <col min="7940" max="7941" width="19.36328125" customWidth="1"/>
     <col min="7950" max="7950" width="10" bestFit="1" customWidth="1"/>
-    <col min="7951" max="7951" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7951" max="7951" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7954" max="7954" width="10" bestFit="1" customWidth="1"/>
-    <col min="7958" max="7958" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7958" max="7958" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7960" max="7960" width="7" customWidth="1"/>
-    <col min="7962" max="7962" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="43.33203125" customWidth="1"/>
-    <col min="8194" max="8194" width="12.6640625" customWidth="1"/>
-    <col min="8195" max="8195" width="19.6640625" customWidth="1"/>
-    <col min="8196" max="8197" width="19.33203125" customWidth="1"/>
+    <col min="7962" max="7962" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="43.36328125" customWidth="1"/>
+    <col min="8194" max="8194" width="12.6328125" customWidth="1"/>
+    <col min="8195" max="8195" width="19.6328125" customWidth="1"/>
+    <col min="8196" max="8197" width="19.36328125" customWidth="1"/>
     <col min="8206" max="8206" width="10" bestFit="1" customWidth="1"/>
-    <col min="8207" max="8207" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8207" max="8207" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8210" max="8210" width="10" bestFit="1" customWidth="1"/>
-    <col min="8214" max="8214" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8214" max="8214" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8216" max="8216" width="7" customWidth="1"/>
-    <col min="8218" max="8218" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="43.33203125" customWidth="1"/>
-    <col min="8450" max="8450" width="12.6640625" customWidth="1"/>
-    <col min="8451" max="8451" width="19.6640625" customWidth="1"/>
-    <col min="8452" max="8453" width="19.33203125" customWidth="1"/>
+    <col min="8218" max="8218" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="43.36328125" customWidth="1"/>
+    <col min="8450" max="8450" width="12.6328125" customWidth="1"/>
+    <col min="8451" max="8451" width="19.6328125" customWidth="1"/>
+    <col min="8452" max="8453" width="19.36328125" customWidth="1"/>
     <col min="8462" max="8462" width="10" bestFit="1" customWidth="1"/>
-    <col min="8463" max="8463" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8463" max="8463" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8466" max="8466" width="10" bestFit="1" customWidth="1"/>
-    <col min="8470" max="8470" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8470" max="8470" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8472" max="8472" width="7" customWidth="1"/>
-    <col min="8474" max="8474" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="43.33203125" customWidth="1"/>
-    <col min="8706" max="8706" width="12.6640625" customWidth="1"/>
-    <col min="8707" max="8707" width="19.6640625" customWidth="1"/>
-    <col min="8708" max="8709" width="19.33203125" customWidth="1"/>
+    <col min="8474" max="8474" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="43.36328125" customWidth="1"/>
+    <col min="8706" max="8706" width="12.6328125" customWidth="1"/>
+    <col min="8707" max="8707" width="19.6328125" customWidth="1"/>
+    <col min="8708" max="8709" width="19.36328125" customWidth="1"/>
     <col min="8718" max="8718" width="10" bestFit="1" customWidth="1"/>
-    <col min="8719" max="8719" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8719" max="8719" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8722" max="8722" width="10" bestFit="1" customWidth="1"/>
-    <col min="8726" max="8726" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8726" max="8726" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8728" max="8728" width="7" customWidth="1"/>
-    <col min="8730" max="8730" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="43.33203125" customWidth="1"/>
-    <col min="8962" max="8962" width="12.6640625" customWidth="1"/>
-    <col min="8963" max="8963" width="19.6640625" customWidth="1"/>
-    <col min="8964" max="8965" width="19.33203125" customWidth="1"/>
+    <col min="8730" max="8730" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="43.36328125" customWidth="1"/>
+    <col min="8962" max="8962" width="12.6328125" customWidth="1"/>
+    <col min="8963" max="8963" width="19.6328125" customWidth="1"/>
+    <col min="8964" max="8965" width="19.36328125" customWidth="1"/>
     <col min="8974" max="8974" width="10" bestFit="1" customWidth="1"/>
-    <col min="8975" max="8975" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8975" max="8975" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8978" max="8978" width="10" bestFit="1" customWidth="1"/>
-    <col min="8982" max="8982" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8982" max="8982" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8984" max="8984" width="7" customWidth="1"/>
-    <col min="8986" max="8986" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="43.33203125" customWidth="1"/>
-    <col min="9218" max="9218" width="12.6640625" customWidth="1"/>
-    <col min="9219" max="9219" width="19.6640625" customWidth="1"/>
-    <col min="9220" max="9221" width="19.33203125" customWidth="1"/>
+    <col min="8986" max="8986" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="43.36328125" customWidth="1"/>
+    <col min="9218" max="9218" width="12.6328125" customWidth="1"/>
+    <col min="9219" max="9219" width="19.6328125" customWidth="1"/>
+    <col min="9220" max="9221" width="19.36328125" customWidth="1"/>
     <col min="9230" max="9230" width="10" bestFit="1" customWidth="1"/>
-    <col min="9231" max="9231" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9231" max="9231" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9234" max="9234" width="10" bestFit="1" customWidth="1"/>
-    <col min="9238" max="9238" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9238" max="9238" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="9240" max="9240" width="7" customWidth="1"/>
-    <col min="9242" max="9242" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="43.33203125" customWidth="1"/>
-    <col min="9474" max="9474" width="12.6640625" customWidth="1"/>
-    <col min="9475" max="9475" width="19.6640625" customWidth="1"/>
-    <col min="9476" max="9477" width="19.33203125" customWidth="1"/>
+    <col min="9242" max="9242" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="43.36328125" customWidth="1"/>
+    <col min="9474" max="9474" width="12.6328125" customWidth="1"/>
+    <col min="9475" max="9475" width="19.6328125" customWidth="1"/>
+    <col min="9476" max="9477" width="19.36328125" customWidth="1"/>
     <col min="9486" max="9486" width="10" bestFit="1" customWidth="1"/>
-    <col min="9487" max="9487" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9487" max="9487" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9490" max="9490" width="10" bestFit="1" customWidth="1"/>
-    <col min="9494" max="9494" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9494" max="9494" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="9496" max="9496" width="7" customWidth="1"/>
-    <col min="9498" max="9498" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="43.33203125" customWidth="1"/>
-    <col min="9730" max="9730" width="12.6640625" customWidth="1"/>
-    <col min="9731" max="9731" width="19.6640625" customWidth="1"/>
-    <col min="9732" max="9733" width="19.33203125" customWidth="1"/>
+    <col min="9498" max="9498" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="43.36328125" customWidth="1"/>
+    <col min="9730" max="9730" width="12.6328125" customWidth="1"/>
+    <col min="9731" max="9731" width="19.6328125" customWidth="1"/>
+    <col min="9732" max="9733" width="19.36328125" customWidth="1"/>
     <col min="9742" max="9742" width="10" bestFit="1" customWidth="1"/>
-    <col min="9743" max="9743" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9743" max="9743" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9746" max="9746" width="10" bestFit="1" customWidth="1"/>
-    <col min="9750" max="9750" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9750" max="9750" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="9752" max="9752" width="7" customWidth="1"/>
-    <col min="9754" max="9754" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="43.33203125" customWidth="1"/>
-    <col min="9986" max="9986" width="12.6640625" customWidth="1"/>
-    <col min="9987" max="9987" width="19.6640625" customWidth="1"/>
-    <col min="9988" max="9989" width="19.33203125" customWidth="1"/>
+    <col min="9754" max="9754" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="43.36328125" customWidth="1"/>
+    <col min="9986" max="9986" width="12.6328125" customWidth="1"/>
+    <col min="9987" max="9987" width="19.6328125" customWidth="1"/>
+    <col min="9988" max="9989" width="19.36328125" customWidth="1"/>
     <col min="9998" max="9998" width="10" bestFit="1" customWidth="1"/>
-    <col min="9999" max="9999" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9999" max="9999" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10002" max="10002" width="10" bestFit="1" customWidth="1"/>
-    <col min="10006" max="10006" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10006" max="10006" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10008" max="10008" width="7" customWidth="1"/>
-    <col min="10010" max="10010" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="43.33203125" customWidth="1"/>
-    <col min="10242" max="10242" width="12.6640625" customWidth="1"/>
-    <col min="10243" max="10243" width="19.6640625" customWidth="1"/>
-    <col min="10244" max="10245" width="19.33203125" customWidth="1"/>
+    <col min="10010" max="10010" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="43.36328125" customWidth="1"/>
+    <col min="10242" max="10242" width="12.6328125" customWidth="1"/>
+    <col min="10243" max="10243" width="19.6328125" customWidth="1"/>
+    <col min="10244" max="10245" width="19.36328125" customWidth="1"/>
     <col min="10254" max="10254" width="10" bestFit="1" customWidth="1"/>
-    <col min="10255" max="10255" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10255" max="10255" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10258" max="10258" width="10" bestFit="1" customWidth="1"/>
-    <col min="10262" max="10262" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10262" max="10262" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10264" max="10264" width="7" customWidth="1"/>
-    <col min="10266" max="10266" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="43.33203125" customWidth="1"/>
-    <col min="10498" max="10498" width="12.6640625" customWidth="1"/>
-    <col min="10499" max="10499" width="19.6640625" customWidth="1"/>
-    <col min="10500" max="10501" width="19.33203125" customWidth="1"/>
+    <col min="10266" max="10266" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="43.36328125" customWidth="1"/>
+    <col min="10498" max="10498" width="12.6328125" customWidth="1"/>
+    <col min="10499" max="10499" width="19.6328125" customWidth="1"/>
+    <col min="10500" max="10501" width="19.36328125" customWidth="1"/>
     <col min="10510" max="10510" width="10" bestFit="1" customWidth="1"/>
-    <col min="10511" max="10511" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10511" max="10511" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10514" max="10514" width="10" bestFit="1" customWidth="1"/>
-    <col min="10518" max="10518" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10518" max="10518" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10520" max="10520" width="7" customWidth="1"/>
-    <col min="10522" max="10522" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="43.33203125" customWidth="1"/>
-    <col min="10754" max="10754" width="12.6640625" customWidth="1"/>
-    <col min="10755" max="10755" width="19.6640625" customWidth="1"/>
-    <col min="10756" max="10757" width="19.33203125" customWidth="1"/>
+    <col min="10522" max="10522" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="43.36328125" customWidth="1"/>
+    <col min="10754" max="10754" width="12.6328125" customWidth="1"/>
+    <col min="10755" max="10755" width="19.6328125" customWidth="1"/>
+    <col min="10756" max="10757" width="19.36328125" customWidth="1"/>
     <col min="10766" max="10766" width="10" bestFit="1" customWidth="1"/>
-    <col min="10767" max="10767" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10767" max="10767" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10770" max="10770" width="10" bestFit="1" customWidth="1"/>
-    <col min="10774" max="10774" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10774" max="10774" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10776" max="10776" width="7" customWidth="1"/>
-    <col min="10778" max="10778" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="43.33203125" customWidth="1"/>
-    <col min="11010" max="11010" width="12.6640625" customWidth="1"/>
-    <col min="11011" max="11011" width="19.6640625" customWidth="1"/>
-    <col min="11012" max="11013" width="19.33203125" customWidth="1"/>
+    <col min="10778" max="10778" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="43.36328125" customWidth="1"/>
+    <col min="11010" max="11010" width="12.6328125" customWidth="1"/>
+    <col min="11011" max="11011" width="19.6328125" customWidth="1"/>
+    <col min="11012" max="11013" width="19.36328125" customWidth="1"/>
     <col min="11022" max="11022" width="10" bestFit="1" customWidth="1"/>
-    <col min="11023" max="11023" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11023" max="11023" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11026" max="11026" width="10" bestFit="1" customWidth="1"/>
-    <col min="11030" max="11030" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11030" max="11030" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11032" max="11032" width="7" customWidth="1"/>
-    <col min="11034" max="11034" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="43.33203125" customWidth="1"/>
-    <col min="11266" max="11266" width="12.6640625" customWidth="1"/>
-    <col min="11267" max="11267" width="19.6640625" customWidth="1"/>
-    <col min="11268" max="11269" width="19.33203125" customWidth="1"/>
+    <col min="11034" max="11034" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="43.36328125" customWidth="1"/>
+    <col min="11266" max="11266" width="12.6328125" customWidth="1"/>
+    <col min="11267" max="11267" width="19.6328125" customWidth="1"/>
+    <col min="11268" max="11269" width="19.36328125" customWidth="1"/>
     <col min="11278" max="11278" width="10" bestFit="1" customWidth="1"/>
-    <col min="11279" max="11279" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11279" max="11279" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11282" max="11282" width="10" bestFit="1" customWidth="1"/>
-    <col min="11286" max="11286" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11286" max="11286" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11288" max="11288" width="7" customWidth="1"/>
-    <col min="11290" max="11290" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="43.33203125" customWidth="1"/>
-    <col min="11522" max="11522" width="12.6640625" customWidth="1"/>
-    <col min="11523" max="11523" width="19.6640625" customWidth="1"/>
-    <col min="11524" max="11525" width="19.33203125" customWidth="1"/>
+    <col min="11290" max="11290" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="43.36328125" customWidth="1"/>
+    <col min="11522" max="11522" width="12.6328125" customWidth="1"/>
+    <col min="11523" max="11523" width="19.6328125" customWidth="1"/>
+    <col min="11524" max="11525" width="19.36328125" customWidth="1"/>
     <col min="11534" max="11534" width="10" bestFit="1" customWidth="1"/>
-    <col min="11535" max="11535" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11535" max="11535" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11538" max="11538" width="10" bestFit="1" customWidth="1"/>
-    <col min="11542" max="11542" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11542" max="11542" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11544" max="11544" width="7" customWidth="1"/>
-    <col min="11546" max="11546" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="43.33203125" customWidth="1"/>
-    <col min="11778" max="11778" width="12.6640625" customWidth="1"/>
-    <col min="11779" max="11779" width="19.6640625" customWidth="1"/>
-    <col min="11780" max="11781" width="19.33203125" customWidth="1"/>
+    <col min="11546" max="11546" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="43.36328125" customWidth="1"/>
+    <col min="11778" max="11778" width="12.6328125" customWidth="1"/>
+    <col min="11779" max="11779" width="19.6328125" customWidth="1"/>
+    <col min="11780" max="11781" width="19.36328125" customWidth="1"/>
     <col min="11790" max="11790" width="10" bestFit="1" customWidth="1"/>
-    <col min="11791" max="11791" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11791" max="11791" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11794" max="11794" width="10" bestFit="1" customWidth="1"/>
-    <col min="11798" max="11798" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11798" max="11798" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11800" max="11800" width="7" customWidth="1"/>
-    <col min="11802" max="11802" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="43.33203125" customWidth="1"/>
-    <col min="12034" max="12034" width="12.6640625" customWidth="1"/>
-    <col min="12035" max="12035" width="19.6640625" customWidth="1"/>
-    <col min="12036" max="12037" width="19.33203125" customWidth="1"/>
+    <col min="11802" max="11802" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="43.36328125" customWidth="1"/>
+    <col min="12034" max="12034" width="12.6328125" customWidth="1"/>
+    <col min="12035" max="12035" width="19.6328125" customWidth="1"/>
+    <col min="12036" max="12037" width="19.36328125" customWidth="1"/>
     <col min="12046" max="12046" width="10" bestFit="1" customWidth="1"/>
-    <col min="12047" max="12047" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12047" max="12047" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12050" max="12050" width="10" bestFit="1" customWidth="1"/>
-    <col min="12054" max="12054" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12054" max="12054" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12056" max="12056" width="7" customWidth="1"/>
-    <col min="12058" max="12058" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="43.33203125" customWidth="1"/>
-    <col min="12290" max="12290" width="12.6640625" customWidth="1"/>
-    <col min="12291" max="12291" width="19.6640625" customWidth="1"/>
-    <col min="12292" max="12293" width="19.33203125" customWidth="1"/>
+    <col min="12058" max="12058" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="43.36328125" customWidth="1"/>
+    <col min="12290" max="12290" width="12.6328125" customWidth="1"/>
+    <col min="12291" max="12291" width="19.6328125" customWidth="1"/>
+    <col min="12292" max="12293" width="19.36328125" customWidth="1"/>
     <col min="12302" max="12302" width="10" bestFit="1" customWidth="1"/>
-    <col min="12303" max="12303" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12303" max="12303" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12306" max="12306" width="10" bestFit="1" customWidth="1"/>
-    <col min="12310" max="12310" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12310" max="12310" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12312" max="12312" width="7" customWidth="1"/>
-    <col min="12314" max="12314" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="43.33203125" customWidth="1"/>
-    <col min="12546" max="12546" width="12.6640625" customWidth="1"/>
-    <col min="12547" max="12547" width="19.6640625" customWidth="1"/>
-    <col min="12548" max="12549" width="19.33203125" customWidth="1"/>
+    <col min="12314" max="12314" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="43.36328125" customWidth="1"/>
+    <col min="12546" max="12546" width="12.6328125" customWidth="1"/>
+    <col min="12547" max="12547" width="19.6328125" customWidth="1"/>
+    <col min="12548" max="12549" width="19.36328125" customWidth="1"/>
     <col min="12558" max="12558" width="10" bestFit="1" customWidth="1"/>
-    <col min="12559" max="12559" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12559" max="12559" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12562" max="12562" width="10" bestFit="1" customWidth="1"/>
-    <col min="12566" max="12566" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12566" max="12566" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12568" max="12568" width="7" customWidth="1"/>
-    <col min="12570" max="12570" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="43.33203125" customWidth="1"/>
-    <col min="12802" max="12802" width="12.6640625" customWidth="1"/>
-    <col min="12803" max="12803" width="19.6640625" customWidth="1"/>
-    <col min="12804" max="12805" width="19.33203125" customWidth="1"/>
+    <col min="12570" max="12570" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="43.36328125" customWidth="1"/>
+    <col min="12802" max="12802" width="12.6328125" customWidth="1"/>
+    <col min="12803" max="12803" width="19.6328125" customWidth="1"/>
+    <col min="12804" max="12805" width="19.36328125" customWidth="1"/>
     <col min="12814" max="12814" width="10" bestFit="1" customWidth="1"/>
-    <col min="12815" max="12815" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12815" max="12815" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12818" max="12818" width="10" bestFit="1" customWidth="1"/>
-    <col min="12822" max="12822" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12822" max="12822" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12824" max="12824" width="7" customWidth="1"/>
-    <col min="12826" max="12826" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="43.33203125" customWidth="1"/>
-    <col min="13058" max="13058" width="12.6640625" customWidth="1"/>
-    <col min="13059" max="13059" width="19.6640625" customWidth="1"/>
-    <col min="13060" max="13061" width="19.33203125" customWidth="1"/>
+    <col min="12826" max="12826" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="43.36328125" customWidth="1"/>
+    <col min="13058" max="13058" width="12.6328125" customWidth="1"/>
+    <col min="13059" max="13059" width="19.6328125" customWidth="1"/>
+    <col min="13060" max="13061" width="19.36328125" customWidth="1"/>
     <col min="13070" max="13070" width="10" bestFit="1" customWidth="1"/>
-    <col min="13071" max="13071" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13071" max="13071" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13074" max="13074" width="10" bestFit="1" customWidth="1"/>
-    <col min="13078" max="13078" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13078" max="13078" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13080" max="13080" width="7" customWidth="1"/>
-    <col min="13082" max="13082" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="43.33203125" customWidth="1"/>
-    <col min="13314" max="13314" width="12.6640625" customWidth="1"/>
-    <col min="13315" max="13315" width="19.6640625" customWidth="1"/>
-    <col min="13316" max="13317" width="19.33203125" customWidth="1"/>
+    <col min="13082" max="13082" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="43.36328125" customWidth="1"/>
+    <col min="13314" max="13314" width="12.6328125" customWidth="1"/>
+    <col min="13315" max="13315" width="19.6328125" customWidth="1"/>
+    <col min="13316" max="13317" width="19.36328125" customWidth="1"/>
     <col min="13326" max="13326" width="10" bestFit="1" customWidth="1"/>
-    <col min="13327" max="13327" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13327" max="13327" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13330" max="13330" width="10" bestFit="1" customWidth="1"/>
-    <col min="13334" max="13334" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13334" max="13334" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13336" max="13336" width="7" customWidth="1"/>
-    <col min="13338" max="13338" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="43.33203125" customWidth="1"/>
-    <col min="13570" max="13570" width="12.6640625" customWidth="1"/>
-    <col min="13571" max="13571" width="19.6640625" customWidth="1"/>
-    <col min="13572" max="13573" width="19.33203125" customWidth="1"/>
+    <col min="13338" max="13338" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="43.36328125" customWidth="1"/>
+    <col min="13570" max="13570" width="12.6328125" customWidth="1"/>
+    <col min="13571" max="13571" width="19.6328125" customWidth="1"/>
+    <col min="13572" max="13573" width="19.36328125" customWidth="1"/>
     <col min="13582" max="13582" width="10" bestFit="1" customWidth="1"/>
-    <col min="13583" max="13583" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13583" max="13583" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13586" max="13586" width="10" bestFit="1" customWidth="1"/>
-    <col min="13590" max="13590" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13590" max="13590" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13592" max="13592" width="7" customWidth="1"/>
-    <col min="13594" max="13594" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="43.33203125" customWidth="1"/>
-    <col min="13826" max="13826" width="12.6640625" customWidth="1"/>
-    <col min="13827" max="13827" width="19.6640625" customWidth="1"/>
-    <col min="13828" max="13829" width="19.33203125" customWidth="1"/>
+    <col min="13594" max="13594" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="43.36328125" customWidth="1"/>
+    <col min="13826" max="13826" width="12.6328125" customWidth="1"/>
+    <col min="13827" max="13827" width="19.6328125" customWidth="1"/>
+    <col min="13828" max="13829" width="19.36328125" customWidth="1"/>
     <col min="13838" max="13838" width="10" bestFit="1" customWidth="1"/>
-    <col min="13839" max="13839" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13839" max="13839" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13842" max="13842" width="10" bestFit="1" customWidth="1"/>
-    <col min="13846" max="13846" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13846" max="13846" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13848" max="13848" width="7" customWidth="1"/>
-    <col min="13850" max="13850" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="43.33203125" customWidth="1"/>
-    <col min="14082" max="14082" width="12.6640625" customWidth="1"/>
-    <col min="14083" max="14083" width="19.6640625" customWidth="1"/>
-    <col min="14084" max="14085" width="19.33203125" customWidth="1"/>
+    <col min="13850" max="13850" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="43.36328125" customWidth="1"/>
+    <col min="14082" max="14082" width="12.6328125" customWidth="1"/>
+    <col min="14083" max="14083" width="19.6328125" customWidth="1"/>
+    <col min="14084" max="14085" width="19.36328125" customWidth="1"/>
     <col min="14094" max="14094" width="10" bestFit="1" customWidth="1"/>
-    <col min="14095" max="14095" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14095" max="14095" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14098" max="14098" width="10" bestFit="1" customWidth="1"/>
-    <col min="14102" max="14102" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14102" max="14102" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14104" max="14104" width="7" customWidth="1"/>
-    <col min="14106" max="14106" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="43.33203125" customWidth="1"/>
-    <col min="14338" max="14338" width="12.6640625" customWidth="1"/>
-    <col min="14339" max="14339" width="19.6640625" customWidth="1"/>
-    <col min="14340" max="14341" width="19.33203125" customWidth="1"/>
+    <col min="14106" max="14106" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="43.36328125" customWidth="1"/>
+    <col min="14338" max="14338" width="12.6328125" customWidth="1"/>
+    <col min="14339" max="14339" width="19.6328125" customWidth="1"/>
+    <col min="14340" max="14341" width="19.36328125" customWidth="1"/>
     <col min="14350" max="14350" width="10" bestFit="1" customWidth="1"/>
-    <col min="14351" max="14351" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14351" max="14351" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14354" max="14354" width="10" bestFit="1" customWidth="1"/>
-    <col min="14358" max="14358" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14358" max="14358" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14360" max="14360" width="7" customWidth="1"/>
-    <col min="14362" max="14362" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="43.33203125" customWidth="1"/>
-    <col min="14594" max="14594" width="12.6640625" customWidth="1"/>
-    <col min="14595" max="14595" width="19.6640625" customWidth="1"/>
-    <col min="14596" max="14597" width="19.33203125" customWidth="1"/>
+    <col min="14362" max="14362" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="43.36328125" customWidth="1"/>
+    <col min="14594" max="14594" width="12.6328125" customWidth="1"/>
+    <col min="14595" max="14595" width="19.6328125" customWidth="1"/>
+    <col min="14596" max="14597" width="19.36328125" customWidth="1"/>
     <col min="14606" max="14606" width="10" bestFit="1" customWidth="1"/>
-    <col min="14607" max="14607" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14607" max="14607" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14610" max="14610" width="10" bestFit="1" customWidth="1"/>
-    <col min="14614" max="14614" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14614" max="14614" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14616" max="14616" width="7" customWidth="1"/>
-    <col min="14618" max="14618" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="43.33203125" customWidth="1"/>
-    <col min="14850" max="14850" width="12.6640625" customWidth="1"/>
-    <col min="14851" max="14851" width="19.6640625" customWidth="1"/>
-    <col min="14852" max="14853" width="19.33203125" customWidth="1"/>
+    <col min="14618" max="14618" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="43.36328125" customWidth="1"/>
+    <col min="14850" max="14850" width="12.6328125" customWidth="1"/>
+    <col min="14851" max="14851" width="19.6328125" customWidth="1"/>
+    <col min="14852" max="14853" width="19.36328125" customWidth="1"/>
     <col min="14862" max="14862" width="10" bestFit="1" customWidth="1"/>
-    <col min="14863" max="14863" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14863" max="14863" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14866" max="14866" width="10" bestFit="1" customWidth="1"/>
-    <col min="14870" max="14870" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14870" max="14870" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14872" max="14872" width="7" customWidth="1"/>
-    <col min="14874" max="14874" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="43.33203125" customWidth="1"/>
-    <col min="15106" max="15106" width="12.6640625" customWidth="1"/>
-    <col min="15107" max="15107" width="19.6640625" customWidth="1"/>
-    <col min="15108" max="15109" width="19.33203125" customWidth="1"/>
+    <col min="14874" max="14874" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="43.36328125" customWidth="1"/>
+    <col min="15106" max="15106" width="12.6328125" customWidth="1"/>
+    <col min="15107" max="15107" width="19.6328125" customWidth="1"/>
+    <col min="15108" max="15109" width="19.36328125" customWidth="1"/>
     <col min="15118" max="15118" width="10" bestFit="1" customWidth="1"/>
-    <col min="15119" max="15119" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15119" max="15119" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15122" max="15122" width="10" bestFit="1" customWidth="1"/>
-    <col min="15126" max="15126" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15126" max="15126" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15128" max="15128" width="7" customWidth="1"/>
-    <col min="15130" max="15130" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="43.33203125" customWidth="1"/>
-    <col min="15362" max="15362" width="12.6640625" customWidth="1"/>
-    <col min="15363" max="15363" width="19.6640625" customWidth="1"/>
-    <col min="15364" max="15365" width="19.33203125" customWidth="1"/>
+    <col min="15130" max="15130" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="43.36328125" customWidth="1"/>
+    <col min="15362" max="15362" width="12.6328125" customWidth="1"/>
+    <col min="15363" max="15363" width="19.6328125" customWidth="1"/>
+    <col min="15364" max="15365" width="19.36328125" customWidth="1"/>
     <col min="15374" max="15374" width="10" bestFit="1" customWidth="1"/>
-    <col min="15375" max="15375" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15375" max="15375" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15378" max="15378" width="10" bestFit="1" customWidth="1"/>
-    <col min="15382" max="15382" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15382" max="15382" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15384" max="15384" width="7" customWidth="1"/>
-    <col min="15386" max="15386" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="43.33203125" customWidth="1"/>
-    <col min="15618" max="15618" width="12.6640625" customWidth="1"/>
-    <col min="15619" max="15619" width="19.6640625" customWidth="1"/>
-    <col min="15620" max="15621" width="19.33203125" customWidth="1"/>
+    <col min="15386" max="15386" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="43.36328125" customWidth="1"/>
+    <col min="15618" max="15618" width="12.6328125" customWidth="1"/>
+    <col min="15619" max="15619" width="19.6328125" customWidth="1"/>
+    <col min="15620" max="15621" width="19.36328125" customWidth="1"/>
     <col min="15630" max="15630" width="10" bestFit="1" customWidth="1"/>
-    <col min="15631" max="15631" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15631" max="15631" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15634" max="15634" width="10" bestFit="1" customWidth="1"/>
-    <col min="15638" max="15638" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15638" max="15638" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15640" max="15640" width="7" customWidth="1"/>
-    <col min="15642" max="15642" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="43.33203125" customWidth="1"/>
-    <col min="15874" max="15874" width="12.6640625" customWidth="1"/>
-    <col min="15875" max="15875" width="19.6640625" customWidth="1"/>
-    <col min="15876" max="15877" width="19.33203125" customWidth="1"/>
+    <col min="15642" max="15642" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="43.36328125" customWidth="1"/>
+    <col min="15874" max="15874" width="12.6328125" customWidth="1"/>
+    <col min="15875" max="15875" width="19.6328125" customWidth="1"/>
+    <col min="15876" max="15877" width="19.36328125" customWidth="1"/>
     <col min="15886" max="15886" width="10" bestFit="1" customWidth="1"/>
-    <col min="15887" max="15887" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15887" max="15887" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15890" max="15890" width="10" bestFit="1" customWidth="1"/>
-    <col min="15894" max="15894" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15894" max="15894" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15896" max="15896" width="7" customWidth="1"/>
-    <col min="15898" max="15898" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="43.33203125" customWidth="1"/>
-    <col min="16130" max="16130" width="12.6640625" customWidth="1"/>
-    <col min="16131" max="16131" width="19.6640625" customWidth="1"/>
-    <col min="16132" max="16133" width="19.33203125" customWidth="1"/>
+    <col min="15898" max="15898" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="43.36328125" customWidth="1"/>
+    <col min="16130" max="16130" width="12.6328125" customWidth="1"/>
+    <col min="16131" max="16131" width="19.6328125" customWidth="1"/>
+    <col min="16132" max="16133" width="19.36328125" customWidth="1"/>
     <col min="16142" max="16142" width="10" bestFit="1" customWidth="1"/>
-    <col min="16143" max="16143" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16143" max="16143" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="16146" max="16146" width="10" bestFit="1" customWidth="1"/>
-    <col min="16150" max="16150" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16150" max="16150" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="16152" max="16152" width="7" customWidth="1"/>
-    <col min="16154" max="16154" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16154" max="16154" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>111</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>116</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>118</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -4521,22 +4521,22 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
     <col min="5" max="6" width="23" customWidth="1"/>
-    <col min="7" max="10" width="15.83203125" customWidth="1"/>
+    <col min="7" max="10" width="15.81640625" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="111.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="111.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>190</v>
       </c>
       <c r="D2" s="19">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="E2" s="19">
         <v>80000</v>
@@ -4668,7 +4668,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -4813,27 +4813,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E588DD75-4ED6-A447-B30A-4A128452EE65}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="8.83203125"/>
+    <col min="13" max="21" width="8.81640625"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" customWidth="1"/>
+    <col min="23" max="23" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>218</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>219</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>220</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="49"/>
       <c r="U7" s="49"/>
     </row>
@@ -5140,16 +5140,16 @@
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="4" max="5" width="21.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>97</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>97</v>
       </c>
@@ -5404,16 +5404,16 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="15" max="15" width="29.6640625" customWidth="1"/>
+    <col min="15" max="15" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -5522,20 +5522,20 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" customWidth="1"/>
-    <col min="23" max="23" width="10.5" customWidth="1"/>
+    <col min="21" max="21" width="14.36328125" customWidth="1"/>
+    <col min="22" max="22" width="12.6328125" customWidth="1"/>
+    <col min="23" max="23" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -5636,7 +5636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -5862,15 +5862,15 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="5" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -5981,21 +5981,21 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="93.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="93.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>147</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>150</v>
       </c>
@@ -6190,10 +6190,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O9" s="11"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O11" s="11"/>
     </row>
   </sheetData>
@@ -6209,21 +6209,21 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>125</v>
       </c>
@@ -6686,10 +6686,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O13" s="11"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O15" s="11"/>
     </row>
   </sheetData>
@@ -6708,20 +6708,20 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
+    <col min="11" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>134</v>
       </c>
@@ -7125,7 +7125,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>135</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>136</v>
       </c>
@@ -7442,23 +7442,23 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="29" customWidth="1"/>
     <col min="22" max="22" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>82</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F6" s="22"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -7808,7 +7808,7 @@
       <c r="L6" s="22"/>
       <c r="V6" s="23"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -7818,7 +7818,7 @@
       <c r="L7" s="22"/>
       <c r="V7" s="26"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
@@ -7827,7 +7827,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
@@ -7836,7 +7836,7 @@
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
@@ -7845,7 +7845,7 @@
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
@@ -7870,26 +7870,26 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="4" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" customWidth="1"/>
-    <col min="16" max="16" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>201</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>201</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>200</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>200</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>200</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>200</v>
       </c>
@@ -8384,7 +8384,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>198</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>198</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>198</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>198</v>
       </c>
@@ -8684,21 +8684,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="11" width="16.5" customWidth="1"/>
-    <col min="18" max="18" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="11" width="16.453125" customWidth="1"/>
+    <col min="18" max="18" width="22.6328125" customWidth="1"/>
     <col min="22" max="22" width="75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>164</v>
       </c>
       <c r="E2" s="19">
-        <v>28000</v>
+        <v>1</v>
       </c>
       <c r="F2" s="19">
         <v>90000</v>
@@ -8834,7 +8834,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>166</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>165</v>
       </c>
       <c r="E5" s="19">
-        <v>28000</v>
+        <v>1</v>
       </c>
       <c r="F5" s="19">
         <v>90000</v>
@@ -9038,7 +9038,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>168</v>
       </c>
@@ -9106,7 +9106,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -9174,7 +9174,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>167</v>
       </c>
@@ -9188,7 +9188,7 @@
         <v>164</v>
       </c>
       <c r="E8" s="19">
-        <v>28000</v>
+        <v>1</v>
       </c>
       <c r="F8" s="19">
         <v>90000</v>
@@ -9242,7 +9242,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>167</v>
       </c>
@@ -9310,7 +9310,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>167</v>
       </c>

</xml_diff>